<commit_message>
multiple forecasts per top offenders - CFs
</commit_message>
<xml_diff>
--- a/Final Report CFs.xlsx
+++ b/Final Report CFs.xlsx
@@ -6029,7 +6029,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6130,6 +6130,17 @@
         <v>0.131977862914509</v>
       </c>
       <c r="C9" s="1">
+        <v>-0.0565708245097057</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>800</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.131977862914509</v>
+      </c>
+      <c r="C10" s="1">
         <v>-0.0565708245097057</v>
       </c>
     </row>

</xml_diff>